<commit_message>
feat seeders and bug
</commit_message>
<xml_diff>
--- a/frontend/assets/database/backup_all.xlsx
+++ b/frontend/assets/database/backup_all.xlsx
@@ -458,16 +458,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bu Sari</t>
+          <t>Zendaya</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Guru kelas 3A dan 3B</t>
+          <t>Guru kelas 5A</t>
         </is>
       </c>
     </row>
@@ -477,7 +477,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Pak Budi</t>
+          <t>Tom Holland</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -492,7 +492,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bu Ani</t>
+          <t>Andrew Garfield</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -503,31 +503,31 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Pak Deni</t>
+          <t>Crystenz Danz</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Guru kelas 5A</t>
+          <t>Guru kelas 5B</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bu Rina</t>
+          <t>Emma Stone</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Guru kelas 5B</t>
+          <t>Guru kelas 3A dan 3B</t>
         </is>
       </c>
     </row>
@@ -699,11 +699,11 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ahmad Rizki</t>
+          <t>Siti Nurhaliza</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -721,25 +721,25 @@
         <v>5</v>
       </c>
       <c r="G2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H2" t="n">
         <v>4</v>
       </c>
       <c r="I2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J2" t="n">
         <v>4</v>
       </c>
       <c r="K2" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L2" t="n">
         <v>5</v>
       </c>
       <c r="M2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N2" t="n">
         <v>5</v>
@@ -748,10 +748,10 @@
         <v>4</v>
       </c>
       <c r="P2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q2" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="R2" t="n">
         <v>5</v>
@@ -760,22 +760,22 @@
         <v>5</v>
       </c>
       <c r="T2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="V2" t="n">
         <v>5</v>
       </c>
       <c r="W2" t="n">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="X2" t="n">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="Y2" t="n">
-        <v>21.67</v>
+        <v>23.67</v>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
@@ -784,28 +784,28 @@
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>Siswa menunjukkan perkembangan yang baik dalam speaking dan kosakata.</t>
+          <t>Siswa sangat aktif dan menunjukkan kemampuan yang sangat baik di semua aspek.</t>
         </is>
       </c>
       <c r="AB2" s="2" t="n">
-        <v>45906.40879212963</v>
+        <v>45907.19290165509</v>
       </c>
       <c r="AC2" s="2" t="n">
-        <v>45906.40879212963</v>
+        <v>45907.19290165509</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Siti Nurhaliza</t>
+          <t>Budi Santoso</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>3B</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -815,110 +815,110 @@
         <v>1</v>
       </c>
       <c r="F3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K3" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="L3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q3" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="R3" t="n">
         <v>5</v>
       </c>
       <c r="S3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V3" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W3" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="X3" t="n">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="Y3" t="n">
-        <v>23.67</v>
+        <v>18.33</v>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>Sangat Baik</t>
+          <t>Baik</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>Siswa sangat aktif dan menunjukkan kemampuan yang sangat baik di semua aspek.</t>
+          <t>Siswa menunjukkan peningkatan bertahap, perlu lebih banyak latihan pengucapan.</t>
         </is>
       </c>
       <c r="AB3" s="2" t="n">
-        <v>45906.40879486111</v>
+        <v>45907.19290210648</v>
       </c>
       <c r="AC3" s="2" t="n">
-        <v>45906.40879486111</v>
+        <v>45907.19290210648</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Budi Santoso</t>
+          <t>Fitri Ramadhani</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>3B</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E4" t="n">
         <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G4" t="n">
         <v>3</v>
       </c>
       <c r="H4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I4" t="n">
         <v>3</v>
@@ -927,25 +927,25 @@
         <v>3</v>
       </c>
       <c r="K4" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M4" t="n">
         <v>4</v>
       </c>
       <c r="N4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P4" t="n">
         <v>4</v>
       </c>
       <c r="Q4" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="R4" t="n">
         <v>5</v>
@@ -966,10 +966,10 @@
         <v>21</v>
       </c>
       <c r="X4" t="n">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="Y4" t="n">
-        <v>18.33</v>
+        <v>20</v>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
@@ -978,362 +978,358 @@
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>Siswa menunjukkan peningkatan bertahap, perlu lebih banyak latihan pengucapan.</t>
+          <t>Siswa rajin hadir dan menunjukkan peningkatan yang konsisten.</t>
         </is>
       </c>
       <c r="AB4" s="2" t="n">
-        <v>45906.40879537037</v>
+        <v>45907.19290434028</v>
       </c>
       <c r="AC4" s="2" t="n">
-        <v>45906.40879537037</v>
+        <v>45907.19290434028</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Dewi Lestari</t>
+          <t>Joko Susilo</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K5" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="L5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N5" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="O5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Q5" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="R5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="U5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="V5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="W5" t="n">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="X5" t="n">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="Y5" t="n">
-        <v>23.67</v>
+        <v>13.33</v>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>Sangat Baik</t>
+          <t>Cukup</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>Siswa sangat berprestasi dan konsisten dalam semua aspek pembelajaran.</t>
+          <t>Siswa memerlukan perhatian khusus dan motivasi tambahan untuk meningkatkan partisipasi.</t>
         </is>
       </c>
       <c r="AB5" s="2" t="n">
-        <v>45906.40879920139</v>
+        <v>45907.19290532407</v>
       </c>
       <c r="AC5" s="2" t="n">
-        <v>45906.40879920139</v>
+        <v>45907.19290532407</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Andi Wijaya</t>
+          <t>Indah Permata</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>4A</t>
+          <t>5B</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E6" t="n">
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J6" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K6" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="L6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q6" t="n">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="R6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="T6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="U6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="V6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="W6" t="n">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="X6" t="n">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="Y6" t="n">
-        <v>15</v>
+        <v>24.67</v>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>Cukup</t>
+          <t>Sangat Baik</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>Siswa perlu bimbingan ekstra, terutama dalam kosakata dan speaking.</t>
+          <t>Siswa sangat berprestasi dan dapat membantu teman-teman yang kesulitan.</t>
         </is>
       </c>
       <c r="AB6" s="2" t="n">
-        <v>45906.40880018519</v>
+        <v>45907.19290578704</v>
       </c>
       <c r="AC6" s="2" t="n">
-        <v>45906.40880018519</v>
+        <v>45907.19290578704</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Maya Sari</t>
+          <t>Andi Wijaya</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>4B</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
       </c>
       <c r="F7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K7" t="n">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="L7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q7" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="R7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S7" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V7" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W7" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="X7" t="n">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="Y7" t="n">
-        <v>21.33</v>
+        <v>15</v>
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>Sangat Baik</t>
-        </is>
-      </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>Siswa stabil dan konsisten, menunjukkan kemampuan yang baik.</t>
-        </is>
-      </c>
+          <t>Cukup</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr"/>
       <c r="AB7" s="2" t="n">
-        <v>45906.40880383102</v>
+        <v>45907.19290296296</v>
       </c>
       <c r="AC7" s="2" t="n">
-        <v>45906.40880383102</v>
+        <v>45907.20727947917</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Rudi Hermawan</t>
+          <t>Ahmad Rizki</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>5A</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E8" t="n">
         <v>1</v>
       </c>
       <c r="F8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I8" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J8" t="n">
         <v>4</v>
       </c>
       <c r="K8" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L8" t="n">
         <v>5</v>
       </c>
       <c r="M8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N8" t="n">
         <v>5</v>
       </c>
       <c r="O8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Q8" t="n">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="R8" t="n">
         <v>5</v>
@@ -1342,47 +1338,43 @@
         <v>5</v>
       </c>
       <c r="T8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V8" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="W8" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="X8" t="n">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="Y8" t="n">
-        <v>24.33</v>
+        <v>20.67</v>
       </c>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>Sangat Baik</t>
-        </is>
-      </c>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>Siswa memiliki kemampuan luar biasa, dapat menjadi contoh untuk teman-teman.</t>
-        </is>
-      </c>
+          <t>Baik</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr"/>
       <c r="AB8" s="2" t="n">
-        <v>45906.40880456018</v>
+        <v>45907.192900625</v>
       </c>
       <c r="AC8" s="2" t="n">
-        <v>45906.40880456018</v>
+        <v>45907.24896291667</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Fitri Ramadhani</t>
+          <t>Rudi Hermawan</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1400,195 +1392,187 @@
         <v>5</v>
       </c>
       <c r="G9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K9" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="L9" t="n">
         <v>5</v>
       </c>
       <c r="M9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P9" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q9" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="R9" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="T9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="W9" t="n">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="X9" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="Y9" t="n">
-        <v>20</v>
+        <v>16.67</v>
       </c>
       <c r="Z9" t="inlineStr">
         <is>
           <t>Baik</t>
         </is>
       </c>
-      <c r="AA9" t="inlineStr">
-        <is>
-          <t>Siswa rajin hadir dan menunjukkan peningkatan yang konsisten.</t>
-        </is>
-      </c>
+      <c r="AA9" t="inlineStr"/>
       <c r="AB9" s="2" t="n">
-        <v>45906.40880818287</v>
+        <v>45907.19290392361</v>
       </c>
       <c r="AC9" s="2" t="n">
-        <v>45906.40880818287</v>
+        <v>45907.25062901621</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Joko Susilo</t>
+          <t>Maya Sari</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>4B</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
       </c>
       <c r="F10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K10" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="L10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O10" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q10" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="R10" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U10" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="W10" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="X10" t="n">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="Y10" t="n">
-        <v>13.33</v>
+        <v>21.67</v>
       </c>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>Cukup</t>
-        </is>
-      </c>
-      <c r="AA10" t="inlineStr">
-        <is>
-          <t>Siswa memerlukan perhatian khusus dan motivasi tambahan untuk meningkatkan partisipasi.</t>
-        </is>
-      </c>
+          <t>Sangat Baik</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr"/>
       <c r="AB10" s="2" t="n">
-        <v>45906.4088086574</v>
+        <v>45907.19290341435</v>
       </c>
       <c r="AC10" s="2" t="n">
-        <v>45906.4088086574</v>
+        <v>45907.25089626158</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Indah Permata</t>
+          <t>tahap 2</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>5B</t>
+          <t>5A</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F11" t="n">
         <v>5</v>
@@ -1600,13 +1584,13 @@
         <v>5</v>
       </c>
       <c r="I11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J11" t="n">
         <v>5</v>
       </c>
       <c r="K11" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L11" t="n">
         <v>5</v>
@@ -1627,29 +1611,29 @@
         <v>25</v>
       </c>
       <c r="R11" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="T11" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="U11" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="V11" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="W11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>50</v>
+      </c>
+      <c r="Y11" t="n">
         <v>25</v>
       </c>
-      <c r="X11" t="n">
-        <v>74</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>24.67</v>
-      </c>
       <c r="Z11" t="inlineStr">
         <is>
           <t>Sangat Baik</t>
@@ -1657,53 +1641,53 @@
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>Siswa sangat berprestasi dan dapat membantu teman-teman yang kesulitan.</t>
+          <t>tahap2</t>
         </is>
       </c>
       <c r="AB11" s="2" t="n">
-        <v>45906.40881086806</v>
+        <v>45911.25347222222</v>
       </c>
       <c r="AC11" s="2" t="n">
-        <v>45906.40881086806</v>
+        <v>45907.32526325231</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>alvinzanuap2</t>
+          <t>Dewi Lestari</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>4A</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" t="n">
         <v>1</v>
       </c>
       <c r="F12" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G12" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H12" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K12" t="n">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="L12" t="n">
         <v>5</v>
@@ -1712,56 +1696,56 @@
         <v>5</v>
       </c>
       <c r="N12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O12" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P12" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q12" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="R12" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="S12" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="T12" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U12" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="V12" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W12" t="n">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="X12" t="n">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="Y12" t="n">
-        <v>14</v>
+        <v>24.67</v>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>Cukup</t>
+          <t>Sangat Baik</t>
         </is>
       </c>
       <c r="AA12" t="inlineStr">
         <is>
-          <t>keren waks</t>
+          <t>Siswa sangat berprestasi dan konsisten dalam semua aspek pembelajaran.</t>
         </is>
       </c>
       <c r="AB12" s="2" t="n">
-        <v>45906.42061832176</v>
+        <v>45907.19290255787</v>
       </c>
       <c r="AC12" s="2" t="n">
-        <v>45906.42061832176</v>
+        <v>45907.26760246528</v>
       </c>
     </row>
   </sheetData>
@@ -1828,7 +1812,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>3263dc02-2e10-46a8-88eb-57ac86c13830</t>
+          <t>965e5a3d-e2e7-4986-930b-85e67d978f96</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1837,7 +1821,7 @@
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>45906.40846180191</v>
+        <v>45907.19287397835</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -1847,7 +1831,7 @@
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" s="2" t="n">
-        <v>45906.40845261807</v>
+        <v>45907.19286892472</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>

</xml_diff>